<commit_message>
Prog-entera: Completa datos del Problema 09.
</commit_message>
<xml_diff>
--- a/programacion-entera/codigos/Datos/Datos_Problema-09.xlsx
+++ b/programacion-entera/codigos/Datos/Datos_Problema-09.xlsx
@@ -8,7 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Contenedores" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Filas" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Columnas" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Locaciones-Deshabilitadas" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Contenedores" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +23,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">Fila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distancia (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LD6</t>
+  </si>
   <si>
     <t xml:space="preserve">Contenedor</t>
   </si>
@@ -41,6 +74,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -62,6 +96,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,9 +148,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -159,409 +206,647 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.3724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="3" t="n">
+        <v>1.219</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <f aca="false">B2 + (A3-1) * 2.438</f>
+        <v>3.657</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <f aca="false">B3 + (A4-1) * 2.438</f>
+        <v>8.533</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <f aca="false">B4 + (A5-1) * 2.438 + 1.2</f>
+        <v>17.047</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <f aca="false">B5 + (A6-1) * 2.438</f>
+        <v>26.799</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <f aca="false">B6 + (A7-1) * 2.438</f>
+        <v>38.989</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>3.029</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <f aca="false">B2 + (A3-1) * 6.058</f>
+        <v>9.087</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <f aca="false">B3 + (A4-1) * 6.058 + 1.2</f>
+        <v>22.403</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <f aca="false">B4 + (A5-1) * 6.058</f>
+        <v>40.577</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <f aca="false">B5 + (A6-1) * 6.058 + 1.2</f>
+        <v>66.009</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <f aca="false">B6 + (A7-1) * 6.058</f>
+        <v>96.299</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <f aca="false">B7 + (A8-1) * 6.058 + 1.2</f>
+        <v>133.847</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <f aca="false">B8 + (A9-1) * 6.058</f>
+        <v>176.253</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.1479591836735"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="n">
         <v>3936</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="9" t="n">
         <v>3031</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="9" t="n">
         <v>5063</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="9" t="n">
         <v>3596</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="9" t="n">
         <v>3053</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="9" t="n">
         <v>2413</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="9" t="n">
         <v>1684</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="9" t="n">
         <v>2669</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="9" t="n">
         <v>3337</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="9" t="n">
         <v>3076</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="9" t="n">
         <v>3779</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="9" t="n">
         <v>5237</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="9" t="n">
         <v>2766</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="n">
+      <c r="B15" s="9" t="n">
         <v>1494</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="9" t="n">
         <v>3313</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="9" t="n">
         <v>4161</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="9" t="n">
         <v>2418</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B19" s="9" t="n">
         <v>1358</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="n">
+      <c r="B20" s="9" t="n">
         <v>4964</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B21" s="9" t="n">
         <v>3794</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="n">
+      <c r="B22" s="9" t="n">
         <v>3633</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+      <c r="A23" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="n">
+      <c r="B23" s="9" t="n">
         <v>4983</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+      <c r="A24" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="n">
+      <c r="B24" s="9" t="n">
         <v>2567</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="n">
+      <c r="B25" s="9" t="n">
         <v>1388</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="n">
+      <c r="B26" s="9" t="n">
         <v>5475</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="A27" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="n">
+      <c r="B27" s="9" t="n">
         <v>3042</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
+      <c r="A28" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="n">
+      <c r="B28" s="9" t="n">
         <v>5385</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+      <c r="A29" s="8" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="n">
+      <c r="B29" s="9" t="n">
         <v>1592</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
+      <c r="A30" s="8" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="n">
+      <c r="B30" s="9" t="n">
         <v>2691</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="n">
+      <c r="B31" s="9" t="n">
         <v>3741</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
+      <c r="A32" s="8" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="n">
+      <c r="B32" s="9" t="n">
         <v>5825</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+      <c r="A33" s="8" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="n">
+      <c r="B33" s="9" t="n">
         <v>3566</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+      <c r="A34" s="8" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="n">
+      <c r="B34" s="9" t="n">
         <v>2675</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+      <c r="A35" s="8" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="n">
+      <c r="B35" s="9" t="n">
         <v>5095</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
+      <c r="A36" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="n">
+      <c r="B36" s="9" t="n">
         <v>2816</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+      <c r="A37" s="8" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="6" t="n">
+      <c r="B37" s="9" t="n">
         <v>3583</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="A38" s="8" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="6" t="n">
+      <c r="B38" s="9" t="n">
         <v>3374</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
+      <c r="A39" s="8" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="6" t="n">
+      <c r="B39" s="9" t="n">
         <v>5053</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
+      <c r="A40" s="8" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="6" t="n">
+      <c r="B40" s="9" t="n">
         <v>3324</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
+      <c r="A41" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="n">
+      <c r="B41" s="9" t="n">
         <v>4542</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="6" t="n">
-        <v>3374</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" s="6" t="n">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="6" t="n">
-        <v>4118</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="6" t="n">
-        <v>4856</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" s="6" t="n">
-        <v>5703</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="B47" s="6" t="n">
-        <v>5960</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="B48" s="6" t="n">
-        <v>5729</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" s="6" t="n">
-        <v>1997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>